<commit_message>
Update - not much progress - Worked on Data Driven method .  So far it doesn't work due to the ACE.OLEDB provider is not registered issue.
</commit_message>
<xml_diff>
--- a/CompanyWebsitePageFactory/TestDataAccess/TestData.xlsx
+++ b/CompanyWebsitePageFactory/TestDataAccess/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9E6274-260C-4C57-9D1D-86CC41822BF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589CB698-7C3F-48D0-94E1-350D0A189AC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="960" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2835" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Key</t>
   </si>
@@ -28,16 +28,31 @@
     <t>SearchTerm</t>
   </si>
   <si>
-    <t>Linklaters</t>
-  </si>
-  <si>
-    <t>InsightsSearch</t>
+    <t>Cyril</t>
+  </si>
+  <si>
+    <t>Cyril Abtan</t>
+  </si>
+  <si>
+    <t>Partial Cyril Abtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyri </t>
+  </si>
+  <si>
+    <t>Surname Cyril Abtan</t>
+  </si>
+  <si>
+    <t>Abtan</t>
+  </si>
+  <si>
+    <t>Firstname Cyricl Abtan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,8 +97,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{B729CC41-6D79-4E1E-AA4A-0F60763CBA0C}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -358,20 +401,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -380,11 +423,35 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>